<commit_message>
Update LinkedIn job posting form via API
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Job_Description</t>
   </si>
@@ -26,6 +26,17 @@
   </si>
   <si>
     <t>Testing Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Develop and simulate ADAS sensors models (camera, radar, lidar, ultrasonic) with in virtual environments.
+• Create and implement test scenarios to validate ADAS features (e.g., AEB, ACC, LKA) Tools like IPG CarMaker.
+• Work closely with vehicle dynamics to ensure accurate integration of dynamics into simulation platforms.
+• Analyze Sensors data and simulation outputs to evaluate features performance and support development.
+• Implement Python programming as required.
+• Participate in Agile development cycles including sprint planning, reviews, and retrospectives
+• Collaborate effectively with team members and stakeholders, maintaining clear and proactive communication
+• Maintain and write clean, scalable, and well-documented code.
+</t>
   </si>
 </sst>
 </file>
@@ -383,7 +394,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -411,6 +422,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add new Job Posting with Job_Id=1 via API
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -1,31 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milan-Prava.MOHANTY\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6999796A-AAB6-4E82-BE36-A6F739EFF8A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>Job_Id</t>
+  </si>
+  <si>
+    <t>Jd_Title</t>
+  </si>
+  <si>
+    <t>Job_Description</t>
+  </si>
+  <si>
+    <t>Total_Years_Min_Exp</t>
+  </si>
+  <si>
+    <t>Total_Years_Max_Exp</t>
+  </si>
+  <si>
+    <t>ML Engineer/Data Scientist</t>
+  </si>
+  <si>
+    <t>Please find the Job Description (JD) below for your reference</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,13 +93,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -91,21 +104,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -143,7 +148,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -177,7 +182,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -212,10 +216,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -388,22 +391,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add new Job Posting with Job_Id=2 via API
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Job_Id</t>
   </si>
@@ -34,7 +34,31 @@
     <t>ML Engineer/Data Scientist</t>
   </si>
   <si>
+    <t>Fullstack Developer</t>
+  </si>
+  <si>
     <t>Please find the Job Description (JD) below for your reference</t>
+  </si>
+  <si>
+    <t>Please find the Job Description (JD) below for your reference.
+Job Role: ML Engineer/Data Scientist
+Job Description:
+• Develop, train, test, and deploy machine learning models across various fields including computer vision, LLMs, and with tabular and time series data.
+• Strong experience in Python, FastAPI, Flask
+• Strong experience in SQL
+• Strong experience Design Pattern/algorithms and data structures
+• Familiarity with OOPS, Design Pattern/algorithms and data structures
+• Familiarity with continuous integration, deployment, and automated build processes for scalable application delivery using Docker/Kubernetes
+• Practical knowledge of one or more major cloud platforms (e.g. Azure, AWS, or GCP).
+• Excellent written and verbal communication skills in English.
+• Experiment with novel deep learning-based technologies such as self-supervised learning and generative AI. 
+• Work directly with customer data and set up data pipelines to collect, curate, transform, and version data. 
+• Participate in the collection, analysis, interpretation, and output of large amounts of data using advanced AI techniques like deep learning, NLP, and computer vision good foundational experience in PyTorch / Tensorflow.
+• Work within the global corporate Artificial Intelligence division, which addresses real business challenges and opportunities across multiple countries.
+• Collaborate across different business and corporate functions in an international team composed of Project Managers, Data Scientists, Data and Software Engineers within the Artificial Intelligence team and others in the Global AI team
+ Qualifications:
+• Bachelor’s degree or master’s degree in data science, Computational Statistics/Mathematics, Computer Science, or related field
+• Fluent English</t>
   </si>
 </sst>
 </file>
@@ -392,7 +416,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -423,13 +447,30 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
         <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new Job Posting with Job_Id=3 via API
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Job_Id</t>
   </si>
@@ -59,6 +59,9 @@
  Qualifications:
 • Bachelor’s degree or master’s degree in data science, Computational Statistics/Mathematics, Computer Science, or related field
 • Fluent English</t>
+  </si>
+  <si>
+    <t>jghvfh</t>
   </si>
 </sst>
 </file>
@@ -416,7 +419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -473,6 +476,23 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=4
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Job_Id</t>
   </si>
@@ -31,10 +31,22 @@
     <t>Total_Years_Max_Exp</t>
   </si>
   <si>
+    <t>Linked_Posted</t>
+  </si>
+  <si>
+    <t>Resume_received</t>
+  </si>
+  <si>
+    <t>Resume_downloaded</t>
+  </si>
+  <si>
     <t>ML Engineer/Data Scientist</t>
   </si>
   <si>
     <t>Fullstack Developer</t>
+  </si>
+  <si>
+    <t>Demo Demo</t>
   </si>
   <si>
     <t>Please find the Job Description (JD) below for your reference</t>
@@ -62,6 +74,9 @@
   </si>
   <si>
     <t>jghvfh</t>
+  </si>
+  <si>
+    <t>DemoDemo</t>
   </si>
 </sst>
 </file>
@@ -419,13 +434,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -441,16 +456,25 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -459,15 +483,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -476,21 +500,47 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
       <c r="E4">
         <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=5
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Job_Id</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>Demo Demo</t>
+  </si>
+  <si>
+    <t>Dotnet Developer</t>
   </si>
   <si>
     <t>Please find the Job Description (JD) below for your reference</t>
@@ -77,6 +80,9 @@
   </si>
   <si>
     <t>DemoDemo</t>
+  </si>
+  <si>
+    <t>Hello</t>
   </si>
 </sst>
 </file>
@@ -434,7 +440,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -474,7 +480,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -491,7 +497,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -508,7 +514,7 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -525,7 +531,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -540,6 +546,32 @@
         <v>0</v>
       </c>
       <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=6
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Job_Id</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>Dotnet Developer</t>
+  </si>
+  <si>
+    <t>Dotnet1 Developer</t>
   </si>
   <si>
     <t>Please find the Job Description (JD) below for your reference</t>
@@ -83,6 +86,9 @@
   </si>
   <si>
     <t>Hello</t>
+  </si>
+  <si>
+    <t>Testing</t>
   </si>
 </sst>
 </file>
@@ -440,7 +446,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -480,7 +486,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -497,7 +503,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -514,7 +520,7 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -531,7 +537,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -557,7 +563,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -572,6 +578,32 @@
         <v>0</v>
       </c>
       <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=7
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Job_Id</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>Dotnet1 Developer</t>
+  </si>
+  <si>
+    <t>ww</t>
   </si>
   <si>
     <t>Please find the Job Description (JD) below for your reference</t>
@@ -446,7 +449,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -486,7 +489,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -503,7 +506,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -520,7 +523,7 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -537,7 +540,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -563,7 +566,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -589,7 +592,7 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -604,6 +607,32 @@
         <v>0</v>
       </c>
       <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=8
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Job_Id</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>ww</t>
+  </si>
+  <si>
+    <t>Testing</t>
   </si>
   <si>
     <t>Please find the Job Description (JD) below for your reference</t>
@@ -89,9 +92,6 @@
   </si>
   <si>
     <t>Hello</t>
-  </si>
-  <si>
-    <t>Testing</t>
   </si>
 </sst>
 </file>
@@ -449,7 +449,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -489,7 +489,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -506,7 +506,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -523,7 +523,7 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -540,7 +540,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -566,7 +566,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -592,7 +592,7 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -633,6 +633,32 @@
         <v>0</v>
       </c>
       <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=9
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Job_Id</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>Testing</t>
+  </si>
+  <si>
+    <t>QA Analyst</t>
   </si>
   <si>
     <t>Please find the Job Description (JD) below for your reference</t>
@@ -92,6 +95,9 @@
   </si>
   <si>
     <t>Hello</t>
+  </si>
+  <si>
+    <t>Testing1</t>
   </si>
 </sst>
 </file>
@@ -449,7 +455,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -489,7 +495,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -506,7 +512,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -523,7 +529,7 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -540,7 +546,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -566,7 +572,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -659,6 +665,32 @@
         <v>0</v>
       </c>
       <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=10
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Job_Id</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>QA Analyst</t>
+  </si>
+  <si>
+    <t>React Developer</t>
   </si>
   <si>
     <t>Please find the Job Description (JD) below for your reference</t>
@@ -98,6 +101,9 @@
   </si>
   <si>
     <t>Testing1</t>
+  </si>
+  <si>
+    <t>dgfsegse</t>
   </si>
 </sst>
 </file>
@@ -455,7 +461,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -495,7 +501,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -512,7 +518,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -529,7 +535,7 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -546,7 +552,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -572,7 +578,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -676,7 +682,7 @@
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -691,6 +697,32 @@
         <v>0</v>
       </c>
       <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=11
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>Job_Id</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>dgfsegse</t>
+  </si>
+  <si>
+    <t>fafwasf</t>
   </si>
 </sst>
 </file>
@@ -461,7 +464,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -726,6 +729,32 @@
         <v>0</v>
       </c>
     </row>
+    <row r="12" spans="1:8">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=12
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Job_Id</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>React Developer</t>
+  </si>
+  <si>
+    <t>Monstack Developer</t>
   </si>
   <si>
     <t>Please find the Job Description (JD) below for your reference</t>
@@ -107,6 +110,9 @@
   </si>
   <si>
     <t>fafwasf</t>
+  </si>
+  <si>
+    <t>Demoo</t>
   </si>
 </sst>
 </file>
@@ -464,7 +470,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -504,7 +510,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -521,7 +527,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -538,7 +544,7 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -555,7 +561,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -581,7 +587,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -685,7 +691,7 @@
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -711,7 +717,7 @@
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -737,7 +743,7 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -752,6 +758,32 @@
         <v>0</v>
       </c>
       <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=13
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Job_Id</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>Monstack Developer</t>
+  </si>
+  <si>
+    <t>Nest JS Developer</t>
   </si>
   <si>
     <t>Please find the Job Description (JD) below for your reference</t>
@@ -113,6 +116,9 @@
   </si>
   <si>
     <t>Demoo</t>
+  </si>
+  <si>
+    <t>Hi</t>
   </si>
 </sst>
 </file>
@@ -470,7 +476,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -510,7 +516,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -527,7 +533,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -544,7 +550,7 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -561,7 +567,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -587,7 +593,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -691,7 +697,7 @@
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -717,7 +723,7 @@
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -743,7 +749,7 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -769,7 +775,7 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -784,6 +790,32 @@
         <v>0</v>
       </c>
       <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=14
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Job_Id</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>Nest JS Developer</t>
+  </si>
+  <si>
+    <t>AI Developer</t>
   </si>
   <si>
     <t>Please find the Job Description (JD) below for your reference</t>
@@ -119,6 +122,9 @@
   </si>
   <si>
     <t>Hi</t>
+  </si>
+  <si>
+    <t>sfef</t>
   </si>
 </sst>
 </file>
@@ -476,7 +482,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -516,7 +522,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -533,7 +539,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -550,7 +556,7 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -567,7 +573,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -593,7 +599,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -697,7 +703,7 @@
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -723,7 +729,7 @@
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -749,7 +755,7 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -775,7 +781,7 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -801,7 +807,7 @@
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -816,6 +822,32 @@
         <v>0</v>
       </c>
       <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=15
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>Job_Id</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>AI Developer</t>
+  </si>
+  <si>
+    <t>Cyber Security Engineer</t>
   </si>
   <si>
     <t>Please find the Job Description (JD) below for your reference</t>
@@ -125,6 +128,9 @@
   </si>
   <si>
     <t>sfef</t>
+  </si>
+  <si>
+    <t>Demo</t>
   </si>
 </sst>
 </file>
@@ -482,7 +488,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -522,7 +528,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -539,7 +545,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -556,7 +562,7 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -573,7 +579,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -599,7 +605,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -703,7 +709,7 @@
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -729,7 +735,7 @@
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -755,7 +761,7 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -781,7 +787,7 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -807,7 +813,7 @@
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -833,7 +839,7 @@
         <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -848,6 +854,32 @@
         <v>0</v>
       </c>
       <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=16
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>Job_Id</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>Cyber Security Engineer</t>
+  </si>
+  <si>
+    <t>stack Developer</t>
   </si>
   <si>
     <t>Please find the Job Description (JD) below for your reference</t>
@@ -131,6 +134,9 @@
   </si>
   <si>
     <t>Demo</t>
+  </si>
+  <si>
+    <t>gggggghfdgf</t>
   </si>
 </sst>
 </file>
@@ -488,7 +494,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -528,7 +534,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -545,7 +551,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -562,7 +568,7 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -579,7 +585,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -605,7 +611,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -709,7 +715,7 @@
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -735,7 +741,7 @@
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -761,7 +767,7 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -787,7 +793,7 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -813,7 +819,7 @@
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -839,7 +845,7 @@
         <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -865,7 +871,7 @@
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -880,6 +886,32 @@
         <v>0</v>
       </c>
       <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=17
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>Job_Id</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>stack Developer</t>
+  </si>
+  <si>
+    <t>Java Developer</t>
   </si>
   <si>
     <t>Please find the Job Description (JD) below for your reference</t>
@@ -137,6 +140,9 @@
   </si>
   <si>
     <t>gggggghfdgf</t>
+  </si>
+  <si>
+    <t>dfdsfsfdsfsd</t>
   </si>
 </sst>
 </file>
@@ -494,7 +500,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -534,7 +540,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -551,7 +557,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -568,7 +574,7 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -585,7 +591,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -611,7 +617,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -715,7 +721,7 @@
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -741,7 +747,7 @@
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -767,7 +773,7 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -793,7 +799,7 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -819,7 +825,7 @@
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -845,7 +851,7 @@
         <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -871,7 +877,7 @@
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -897,7 +903,7 @@
         <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -912,6 +918,32 @@
         <v>0</v>
       </c>
       <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=JD_018
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>Job_Id</t>
   </si>
@@ -40,6 +40,9 @@
     <t>Resume_downloaded</t>
   </si>
   <si>
+    <t>JD_018</t>
+  </si>
+  <si>
     <t>ML Engineer/Data Scientist</t>
   </si>
   <si>
@@ -83,6 +86,9 @@
   </si>
   <si>
     <t>Java Developer</t>
+  </si>
+  <si>
+    <t>Dummy</t>
   </si>
   <si>
     <t>Please find the Job Description (JD) below for your reference</t>
@@ -143,6 +149,9 @@
   </si>
   <si>
     <t>dfdsfsfdsfsd</t>
+  </si>
+  <si>
+    <t>ekhwkqf eurkge</t>
   </si>
 </sst>
 </file>
@@ -500,7 +509,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -537,10 +546,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -554,10 +563,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -571,10 +580,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -588,10 +597,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -614,10 +623,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -640,10 +649,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -666,10 +675,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -692,10 +701,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -718,10 +727,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -744,10 +753,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -770,10 +779,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -796,10 +805,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -822,10 +831,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -848,10 +857,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -874,10 +883,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -900,10 +909,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -926,10 +935,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -944,6 +953,32 @@
         <v>0</v>
       </c>
       <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=JD_001
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -1,27 +1,59 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milan-Prava.MOHANTY\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19DEF100-6EC9-4502-92A4-F649925A9565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>Job_Id</t>
+  </si>
+  <si>
+    <t>Job_Title</t>
+  </si>
+  <si>
+    <t>Job_Description</t>
+  </si>
+  <si>
+    <t>Total_Years_Min_Exp</t>
+  </si>
+  <si>
+    <t>Total_Years_Max_Exp</t>
+  </si>
+  <si>
+    <t>Linked_Posted</t>
+  </si>
+  <si>
+    <t>Resume_received</t>
+  </si>
+  <si>
+    <t>Resume_downloaded</t>
+  </si>
+  <si>
+    <t>JD_001</t>
+  </si>
+  <si>
+    <t>Senior Engineer</t>
+  </si>
+  <si>
+    <t>We are seeking a Software Engineer to build and maintain high-quality software solutions</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,13 +105,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -87,21 +116,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -139,7 +160,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -173,7 +194,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -208,10 +228,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -384,22 +403,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=JD_002
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Job_Id</t>
   </si>
@@ -43,10 +43,20 @@
     <t>JD_001</t>
   </si>
   <si>
+    <t>JD_002</t>
+  </si>
+  <si>
     <t>Senior Engineer</t>
   </si>
   <si>
+    <t>Junior RPA Developer</t>
+  </si>
+  <si>
     <t>We are seeking a Software Engineer to build and maintain high-quality software solutions</t>
+  </si>
+  <si>
+    <t>We are seeking a Junior RPA Developer to design, develop, and support automation solutions.
+Collaborate with teams to streamline business processes using RPA tools like UiPath or Automation Anywhere. Join Akkodis to grow your skills in a dynamic, tech-driven environment</t>
   </si>
 </sst>
 </file>
@@ -404,7 +414,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -441,10 +451,10 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -459,6 +469,32 @@
         <v>0</v>
       </c>
       <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=JD_003
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Job_Id</t>
   </si>
@@ -40,16 +40,25 @@
     <t>Resume_downloaded</t>
   </si>
   <si>
+    <t>Linked_Poster</t>
+  </si>
+  <si>
     <t>JD_001</t>
   </si>
   <si>
     <t>JD_002</t>
   </si>
   <si>
+    <t>JD_003</t>
+  </si>
+  <si>
     <t>Senior Engineer</t>
   </si>
   <si>
     <t>Junior RPA Developer</t>
+  </si>
+  <si>
+    <t>Senior Dotnet Engineer</t>
   </si>
   <si>
     <t>We are seeking a Software Engineer to build and maintain high-quality software solutions</t>
@@ -57,6 +66,11 @@
   <si>
     <t>We are seeking a Junior RPA Developer to design, develop, and support automation solutions.
 Collaborate with teams to streamline business processes using RPA tools like UiPath or Automation Anywhere. Join Akkodis to grow your skills in a dynamic, tech-driven environment</t>
+  </si>
+  <si>
+    <t>We are seeking a Software Engineer to build and maintain high-quality software solutions.
+Work with global teams to drive innovation and deliver scalable applications.
+Join Akkodis and be part of a tech-driven, collaborative environment.</t>
   </si>
 </sst>
 </file>
@@ -414,13 +428,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -445,16 +459,19 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -472,15 +489,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -495,6 +512,35 @@
         <v>0</v>
       </c>
       <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=JD_004
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Job_Id</t>
   </si>
@@ -52,6 +52,9 @@
     <t>JD_003</t>
   </si>
   <si>
+    <t>JD_004</t>
+  </si>
+  <si>
     <t>Senior Engineer</t>
   </si>
   <si>
@@ -59,6 +62,9 @@
   </si>
   <si>
     <t>Junior RPA Developer</t>
+  </si>
+  <si>
+    <t>Senior RPA Developer</t>
   </si>
   <si>
     <t>We are seeking a Software Engineer to build and maintain high-quality software solutions.
@@ -425,7 +431,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -465,10 +471,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -494,10 +500,10 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -523,10 +529,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -544,6 +550,35 @@
         <v>0</v>
       </c>
       <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=JD_005
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Job_Id</t>
   </si>
@@ -55,6 +55,9 @@
     <t>JD_004</t>
   </si>
   <si>
+    <t>JD_005</t>
+  </si>
+  <si>
     <t>Senior Engineer</t>
   </si>
   <si>
@@ -65,6 +68,9 @@
   </si>
   <si>
     <t>Senior RPA Developer</t>
+  </si>
+  <si>
+    <t>Dummy Engineer</t>
   </si>
   <si>
     <t>We are seeking a Software Engineer to build and maintain high-quality software solutions.
@@ -74,6 +80,9 @@
   <si>
     <t>We are seeking a Junior RPA Developer to design, develop, and support automation solutions.
 Collaborate with teams to streamline business processes using RPA tools like UiPath or Automation Anywhere. Join Akkodis to grow your skills in a dynamic, tech-driven environment</t>
+  </si>
+  <si>
+    <t>Dummy Data</t>
   </si>
 </sst>
 </file>
@@ -431,7 +440,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -471,10 +480,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -500,10 +509,10 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -529,10 +538,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -558,10 +567,10 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -580,6 +589,23 @@
       </c>
       <c r="I5">
         <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=JD_006
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Job_Id</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>JD_005</t>
+  </si>
+  <si>
+    <t>JD_006</t>
   </si>
   <si>
     <t>Senior Engineer</t>
@@ -83,6 +86,9 @@
   </si>
   <si>
     <t>Dummy Data</t>
+  </si>
+  <si>
+    <t>dsfdsf</t>
   </si>
 </sst>
 </file>
@@ -440,7 +446,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -480,10 +486,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -509,10 +515,10 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -538,10 +544,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -567,10 +573,10 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -596,16 +602,33 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6">
         <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=JD_007
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Job_Id</t>
   </si>
@@ -61,6 +61,9 @@
     <t>JD_006</t>
   </si>
   <si>
+    <t>JD_007</t>
+  </si>
+  <si>
     <t>Senior Engineer</t>
   </si>
   <si>
@@ -77,6 +80,9 @@
   </si>
   <si>
     <t>Senior IT Engineer</t>
+  </si>
+  <si>
+    <t>Senior Devops Developer</t>
   </si>
   <si>
     <t>We are seeking a Software Engineer to build and maintain high-quality software solutions.
@@ -448,7 +454,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -488,10 +494,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -505,10 +511,10 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -522,10 +528,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -539,10 +545,10 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -556,10 +562,10 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -573,16 +579,33 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D7">
         <v>5</v>
       </c>
       <c r="E7">
         <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=JD_008
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Job_Id</t>
   </si>
@@ -64,6 +64,9 @@
     <t>JD_007</t>
   </si>
   <si>
+    <t>JD_008</t>
+  </si>
+  <si>
     <t>Senior Engineer</t>
   </si>
   <si>
@@ -83,6 +86,9 @@
   </si>
   <si>
     <t>Senior Devops Developer</t>
+  </si>
+  <si>
+    <t>Senior System Engineer</t>
   </si>
   <si>
     <t>We are seeking a Software Engineer to build and maintain high-quality software solutions.
@@ -454,7 +460,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -494,10 +500,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -511,10 +517,10 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -528,10 +534,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -545,10 +551,10 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -562,10 +568,10 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -579,10 +585,10 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -596,16 +602,33 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8">
         <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=JD_009
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Job_Id</t>
   </si>
@@ -67,6 +67,9 @@
     <t>JD_008</t>
   </si>
   <si>
+    <t>JD_009</t>
+  </si>
+  <si>
     <t>Senior Engineer</t>
   </si>
   <si>
@@ -89,6 +92,9 @@
   </si>
   <si>
     <t>Senior System Engineer</t>
+  </si>
+  <si>
+    <t>Senior Test Engineer</t>
   </si>
   <si>
     <t>We are seeking a Software Engineer to build and maintain high-quality software solutions.
@@ -460,7 +466,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -500,10 +506,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -517,10 +523,10 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -534,10 +540,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -551,10 +557,10 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -568,10 +574,10 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -585,10 +591,10 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -602,10 +608,10 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -619,16 +625,33 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
       <c r="E9">
         <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=JD_010
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>Job_Id</t>
   </si>
@@ -70,6 +70,9 @@
     <t>JD_009</t>
   </si>
   <si>
+    <t>JD_010</t>
+  </si>
+  <si>
     <t>Senior Engineer</t>
   </si>
   <si>
@@ -95,6 +98,9 @@
   </si>
   <si>
     <t>Senior Test Engineer</t>
+  </si>
+  <si>
+    <t>Senior Azure Engineer</t>
   </si>
   <si>
     <t>We are seeking a Software Engineer to build and maintain high-quality software solutions.
@@ -466,7 +472,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -506,10 +512,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -523,10 +529,10 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -540,10 +546,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -557,10 +563,10 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -574,10 +580,10 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -591,10 +597,10 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -608,10 +614,10 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -625,10 +631,10 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -642,16 +648,33 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D10">
         <v>5</v>
       </c>
       <c r="E10">
         <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=JD_011
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>Job_Id</t>
   </si>
@@ -73,6 +73,9 @@
     <t>JD_010</t>
   </si>
   <si>
+    <t>JD_011</t>
+  </si>
+  <si>
     <t>Senior Engineer</t>
   </si>
   <si>
@@ -101,6 +104,9 @@
   </si>
   <si>
     <t>Senior Azure Engineer</t>
+  </si>
+  <si>
+    <t>Senior SW Engineer</t>
   </si>
   <si>
     <t>We are seeking a Software Engineer to build and maintain high-quality software solutions.
@@ -472,7 +478,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -512,10 +518,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -529,10 +535,10 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -546,10 +552,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -563,10 +569,10 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -580,10 +586,10 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -597,10 +603,10 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -614,10 +620,10 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -631,10 +637,10 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -648,10 +654,10 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -665,16 +671,33 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
       <c r="E11">
         <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=JD_012
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>Job_Id</t>
   </si>
@@ -76,6 +76,9 @@
     <t>JD_011</t>
   </si>
   <si>
+    <t>JD_012</t>
+  </si>
+  <si>
     <t>Senior Engineer</t>
   </si>
   <si>
@@ -107,6 +110,9 @@
   </si>
   <si>
     <t>Senior SW Engineer</t>
+  </si>
+  <si>
+    <t>Junior Developer</t>
   </si>
   <si>
     <t>We are seeking a Software Engineer to build and maintain high-quality software solutions.
@@ -478,7 +484,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -518,10 +524,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -535,10 +541,10 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -552,10 +558,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -569,10 +575,10 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -586,10 +592,10 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -603,10 +609,10 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -620,10 +626,10 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -637,10 +643,10 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -654,10 +660,10 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -671,10 +677,10 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -688,16 +694,33 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12">
         <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=JD_013
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t>Job_Id</t>
   </si>
@@ -79,6 +79,9 @@
     <t>JD_012</t>
   </si>
   <si>
+    <t>JD_013</t>
+  </si>
+  <si>
     <t>Senior Engineer</t>
   </si>
   <si>
@@ -113,6 +116,9 @@
   </si>
   <si>
     <t>Junior Developer</t>
+  </si>
+  <si>
+    <t>Senior Python Engineer</t>
   </si>
   <si>
     <t>We are seeking a Software Engineer to build and maintain high-quality software solutions.
@@ -484,7 +490,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -524,10 +530,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -541,10 +547,10 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -558,10 +564,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -575,10 +581,10 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -592,10 +598,10 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -609,10 +615,10 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -626,10 +632,10 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -643,10 +649,10 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -660,10 +666,10 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -677,10 +683,10 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -694,10 +700,10 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -711,16 +717,33 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13">
         <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=JD_014
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t>Job_Id</t>
   </si>
@@ -82,6 +82,9 @@
     <t>JD_013</t>
   </si>
   <si>
+    <t>JD_014</t>
+  </si>
+  <si>
     <t>Senior Engineer</t>
   </si>
   <si>
@@ -119,6 +122,9 @@
   </si>
   <si>
     <t>Senior Python Engineer</t>
+  </si>
+  <si>
+    <t>Junior Devops Developer</t>
   </si>
   <si>
     <t>We are seeking a Software Engineer to build and maintain high-quality software solutions.
@@ -490,7 +496,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -530,10 +536,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -547,10 +553,10 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -564,10 +570,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -581,10 +587,10 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -598,10 +604,10 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -615,10 +621,10 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -632,10 +638,10 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -649,10 +655,10 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -666,10 +672,10 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -683,10 +689,10 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -700,10 +706,10 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -717,10 +723,10 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -734,16 +740,33 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14">
         <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=JD_015
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
   <si>
     <t>Job_Id</t>
   </si>
@@ -85,6 +85,9 @@
     <t>JD_014</t>
   </si>
   <si>
+    <t>JD_015</t>
+  </si>
+  <si>
     <t>Senior Engineer</t>
   </si>
   <si>
@@ -125,6 +128,9 @@
   </si>
   <si>
     <t>Junior Devops Developer</t>
+  </si>
+  <si>
+    <t>Junior Dotnet Engineer</t>
   </si>
   <si>
     <t>We are seeking a Software Engineer to build and maintain high-quality software solutions.
@@ -496,7 +502,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -536,10 +542,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -553,10 +559,10 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -570,10 +576,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -587,10 +593,10 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -604,10 +610,10 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -621,10 +627,10 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -638,10 +644,10 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -655,10 +661,10 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -672,10 +678,10 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -689,10 +695,10 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -706,10 +712,10 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -723,10 +729,10 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -740,10 +746,10 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -757,16 +763,33 @@
         <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D15">
         <v>2</v>
       </c>
       <c r="E15">
         <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=JD_016
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
   <si>
     <t>Job_Id</t>
   </si>
@@ -88,6 +88,9 @@
     <t>JD_015</t>
   </si>
   <si>
+    <t>JD_016</t>
+  </si>
+  <si>
     <t>Senior Engineer</t>
   </si>
   <si>
@@ -131,6 +134,9 @@
   </si>
   <si>
     <t>Junior Dotnet Engineer</t>
+  </si>
+  <si>
+    <t>Junior Python Engineer</t>
   </si>
   <si>
     <t>We are seeking a Software Engineer to build and maintain high-quality software solutions.
@@ -502,7 +508,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -542,10 +548,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -559,10 +565,10 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -576,10 +582,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -593,10 +599,10 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -610,10 +616,10 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -627,10 +633,10 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -644,10 +650,10 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -661,10 +667,10 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -678,10 +684,10 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -695,10 +701,10 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -712,10 +718,10 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -729,10 +735,10 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -746,10 +752,10 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -763,10 +769,10 @@
         <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -780,16 +786,33 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D16">
         <v>2</v>
       </c>
       <c r="E16">
         <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=JD_017
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t>Job_Id</t>
   </si>
@@ -91,6 +91,9 @@
     <t>JD_016</t>
   </si>
   <si>
+    <t>JD_017</t>
+  </si>
+  <si>
     <t>Senior Engineer</t>
   </si>
   <si>
@@ -137,6 +140,9 @@
   </si>
   <si>
     <t>Junior Python Engineer</t>
+  </si>
+  <si>
+    <t>Junior AI Developer</t>
   </si>
   <si>
     <t>We are seeking a Software Engineer to build and maintain high-quality software solutions.
@@ -508,7 +514,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -548,10 +554,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -565,10 +571,10 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -582,10 +588,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -599,10 +605,10 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -616,10 +622,10 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -633,10 +639,10 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -650,10 +656,10 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -667,10 +673,10 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -684,10 +690,10 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -701,10 +707,10 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -718,10 +724,10 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -735,10 +741,10 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -752,10 +758,10 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -769,10 +775,10 @@
         <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -786,10 +792,10 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -803,15 +809,32 @@
         <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=JD_019
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
   <si>
     <t>Job_Id</t>
   </si>
@@ -97,6 +97,9 @@
     <t>JD_018</t>
   </si>
   <si>
+    <t>JD_019</t>
+  </si>
+  <si>
     <t>Senior Engineer</t>
   </si>
   <si>
@@ -149,6 +152,9 @@
   </si>
   <si>
     <t>Senior UI Engineer</t>
+  </si>
+  <si>
+    <t>Senior QA Analyst</t>
   </si>
   <si>
     <t>We are seeking a Software Engineer to build and maintain high-quality software solutions.
@@ -520,7 +526,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -560,10 +566,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -577,10 +583,10 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -594,10 +600,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -611,10 +617,10 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -628,10 +634,10 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -645,10 +651,10 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -662,10 +668,10 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -679,10 +685,10 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -696,10 +702,10 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -713,10 +719,10 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -730,10 +736,10 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -747,10 +753,10 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -764,10 +770,10 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -781,10 +787,10 @@
         <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -798,10 +804,10 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -815,10 +821,10 @@
         <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -832,10 +838,10 @@
         <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -849,15 +855,32 @@
         <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D19">
         <v>2</v>
       </c>
       <c r="E19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=JD_020
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
   <si>
     <t>Job_Id</t>
   </si>
@@ -100,6 +100,9 @@
     <t>JD_019</t>
   </si>
   <si>
+    <t>JD_020</t>
+  </si>
+  <si>
     <t>Senior Engineer</t>
   </si>
   <si>
@@ -155,6 +158,9 @@
   </si>
   <si>
     <t>Senior QA Analyst</t>
+  </si>
+  <si>
+    <t>Senior System Analyst</t>
   </si>
   <si>
     <t>We are seeking a Software Engineer to build and maintain high-quality software solutions.
@@ -526,7 +532,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -566,10 +572,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -583,10 +589,10 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -600,10 +606,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -617,10 +623,10 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -634,10 +640,10 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -651,10 +657,10 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -668,10 +674,10 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -685,10 +691,10 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -702,10 +708,10 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -719,10 +725,10 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -736,10 +742,10 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -753,10 +759,10 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -770,10 +776,10 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -787,10 +793,10 @@
         <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -804,10 +810,10 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -821,10 +827,10 @@
         <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -838,10 +844,10 @@
         <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -855,10 +861,10 @@
         <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -872,16 +878,33 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20">
         <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=JD_021
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
   <si>
     <t>Job_Id</t>
   </si>
@@ -103,6 +103,9 @@
     <t>JD_020</t>
   </si>
   <si>
+    <t>JD_021</t>
+  </si>
+  <si>
     <t>Senior Engineer</t>
   </si>
   <si>
@@ -161,6 +164,9 @@
   </si>
   <si>
     <t>Senior System Analyst</t>
+  </si>
+  <si>
+    <t>ASpice Engineer</t>
   </si>
   <si>
     <t>We are seeking a Software Engineer to build and maintain high-quality software solutions.
@@ -532,7 +538,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -572,10 +578,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -589,10 +595,10 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -606,10 +612,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -623,10 +629,10 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -640,10 +646,10 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -657,10 +663,10 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -674,10 +680,10 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -691,10 +697,10 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -708,10 +714,10 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -725,10 +731,10 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -742,10 +748,10 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -759,10 +765,10 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -776,10 +782,10 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -793,10 +799,10 @@
         <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -810,10 +816,10 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -827,10 +833,10 @@
         <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -844,10 +850,10 @@
         <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -861,10 +867,10 @@
         <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -878,10 +884,10 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -895,16 +901,33 @@
         <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C21" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D21">
         <v>2</v>
       </c>
       <c r="E21">
         <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=JD_022
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
   <si>
     <t>Job_Id</t>
   </si>
@@ -106,6 +106,9 @@
     <t>JD_021</t>
   </si>
   <si>
+    <t>JD_022</t>
+  </si>
+  <si>
     <t>Senior Engineer</t>
   </si>
   <si>
@@ -167,6 +170,9 @@
   </si>
   <si>
     <t>ASpice Engineer</t>
+  </si>
+  <si>
+    <t>Mid Engineer</t>
   </si>
   <si>
     <t>We are seeking a Software Engineer to build and maintain high-quality software solutions.
@@ -538,7 +544,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -578,10 +584,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -595,10 +601,10 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -612,10 +618,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -629,10 +635,10 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -646,10 +652,10 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -663,10 +669,10 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -680,10 +686,10 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -697,10 +703,10 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -714,10 +720,10 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -731,10 +737,10 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -748,10 +754,10 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -765,10 +771,10 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -782,10 +788,10 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -799,10 +805,10 @@
         <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -816,10 +822,10 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -833,10 +839,10 @@
         <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -850,10 +856,10 @@
         <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -867,10 +873,10 @@
         <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -884,10 +890,10 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -901,10 +907,10 @@
         <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D21">
         <v>2</v>
@@ -918,16 +924,33 @@
         <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C22" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22">
         <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=JD_023
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="58">
   <si>
     <t>Job_Id</t>
   </si>
@@ -109,6 +109,9 @@
     <t>JD_022</t>
   </si>
   <si>
+    <t>JD_023</t>
+  </si>
+  <si>
     <t>Senior Engineer</t>
   </si>
   <si>
@@ -173,6 +176,9 @@
   </si>
   <si>
     <t>Mid Engineer</t>
+  </si>
+  <si>
+    <t>Junior React Engineer</t>
   </si>
   <si>
     <t>We are seeking a Software Engineer to build and maintain high-quality software solutions.
@@ -544,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -584,10 +590,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -601,10 +607,10 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -618,10 +624,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -635,10 +641,10 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -652,10 +658,10 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -669,10 +675,10 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -686,10 +692,10 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -703,10 +709,10 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -720,10 +726,10 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -737,10 +743,10 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -754,10 +760,10 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -771,10 +777,10 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -788,10 +794,10 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -805,10 +811,10 @@
         <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -822,10 +828,10 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -839,10 +845,10 @@
         <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -856,10 +862,10 @@
         <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -873,10 +879,10 @@
         <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -890,10 +896,10 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C20" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -907,10 +913,10 @@
         <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D21">
         <v>2</v>
@@ -924,10 +930,10 @@
         <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C22" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -941,15 +947,32 @@
         <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=JD_024
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="60">
   <si>
     <t>Job_Id</t>
   </si>
@@ -112,6 +112,9 @@
     <t>JD_023</t>
   </si>
   <si>
+    <t>JD_024</t>
+  </si>
+  <si>
     <t>Senior Engineer</t>
   </si>
   <si>
@@ -179,6 +182,9 @@
   </si>
   <si>
     <t>Junior React Engineer</t>
+  </si>
+  <si>
+    <t>string</t>
   </si>
   <si>
     <t>We are seeking a Software Engineer to build and maintain high-quality software solutions.
@@ -550,7 +556,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -590,10 +596,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -607,10 +613,10 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -624,10 +630,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -641,10 +647,10 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -658,10 +664,10 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -675,10 +681,10 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -692,10 +698,10 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -709,10 +715,10 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -726,10 +732,10 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -743,10 +749,10 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -760,10 +766,10 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -777,10 +783,10 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -794,10 +800,10 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -811,10 +817,10 @@
         <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -828,10 +834,10 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -845,10 +851,10 @@
         <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -862,10 +868,10 @@
         <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -879,10 +885,10 @@
         <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -896,10 +902,10 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -913,10 +919,10 @@
         <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D21">
         <v>2</v>
@@ -930,10 +936,10 @@
         <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -947,10 +953,10 @@
         <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -964,16 +970,33 @@
         <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C24" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24">
         <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Job Posting with Job_Id=JD_025
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="63">
   <si>
     <t>Job_Id</t>
   </si>
@@ -115,6 +115,9 @@
     <t>JD_024</t>
   </si>
   <si>
+    <t>JD_025</t>
+  </si>
+  <si>
     <t>Senior Engineer</t>
   </si>
   <si>
@@ -185,6 +188,9 @@
   </si>
   <si>
     <t>Mid Fullstack Developer</t>
+  </si>
+  <si>
+    <t>Senior Associate Engineer</t>
   </si>
   <si>
     <t>We are seeking a Software Engineer to build and maintain high-quality software solutions.
@@ -199,6 +205,9 @@
     <t xml:space="preserve">We are seeking a Junior RPA Developer to design, develop, and support automation solutions.
 Collaborate with teams to streamline business processes using RPA tools like UiPath or Automation Anywhere. Join Akkodis to grow your skills in a dynamic, tech-driven environment
 </t>
+  </si>
+  <si>
+    <t>Testing</t>
   </si>
 </sst>
 </file>
@@ -556,7 +565,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -596,10 +605,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -613,10 +622,10 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -630,10 +639,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -647,10 +656,10 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -664,10 +673,10 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -681,10 +690,10 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -698,10 +707,10 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -715,10 +724,10 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -732,10 +741,10 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -749,10 +758,10 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -766,10 +775,10 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -783,10 +792,10 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -800,10 +809,10 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -817,10 +826,10 @@
         <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -834,10 +843,10 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -851,10 +860,10 @@
         <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -868,10 +877,10 @@
         <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -885,10 +894,10 @@
         <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -902,10 +911,10 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -919,10 +928,10 @@
         <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D21">
         <v>2</v>
@@ -936,10 +945,10 @@
         <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -953,10 +962,10 @@
         <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C23" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -970,10 +979,10 @@
         <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C24" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -987,16 +996,33 @@
         <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25">
         <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Upload LinkedIn job posting file
</commit_message>
<xml_diff>
--- a/LinkedIn_job_posting.xlsx
+++ b/LinkedIn_job_posting.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sivaprasadh.AJITHA-K\Documents\JOB_PORTAL_AUTOMATION\Linkedin automation\Input file\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3EAFA18-AE2D-4979-B2CA-986E4DAC4BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="2880" yWindow="2810" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Job_Id</t>
   </si>
@@ -79,13 +85,19 @@
     <t xml:space="preserve">We are seeking a Junior RPA Developer to design, develop, and support automation solutions.
 Collaborate with teams to streamline business processes using RPA tools like UiPath or Automation Anywhere. Join Akkodis to grow your skills in a dynamic, tech-driven environment
 </t>
+  </si>
+  <si>
+    <t>Created</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,13 +160,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -192,7 +212,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -226,6 +246,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -260,9 +281,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -435,14 +457,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -471,7 +495,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -487,8 +511,14 @@
       <c r="E2">
         <v>4</v>
       </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -505,7 +535,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -522,7 +552,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>

</xml_diff>